<commit_message>
Ajustes rotinas TRTs, Jusbrasil
</commit_message>
<xml_diff>
--- a/Data/Input/Input_Recursal.xlsx
+++ b/Data/Input/Input_Recursal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafael.lima\Documents\UiPath\Ive_Recursal\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C651D1-9114-4288-954C-6EA703E14313}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEF33DB-052B-4181-B8BA-4CCF810FE680}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="0" activeTab="0" xr2:uid="{35B38B0C-BB26-4715-8F62-F8601697CDBD}"/>
   </x:bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <x:si>
     <x:t>CNPJ</x:t>
   </x:si>
@@ -91,7 +91,13 @@
     <x:t>vml2021</x:t>
   </x:si>
   <x:si>
-    <x:t>BAIXADO</x:t>
+    <x:t>61.603.387/0001-65</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CENTRO SANEAMENTO E SERVIÇOS AVANÇADOS S.A.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INICIAR</x:t>
   </x:si>
   <x:si>
     <x:t>CNPJ da empresa que será verificada</x:t>
@@ -294,7 +300,7 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="67">
+  <x:cellStyleXfs count="41">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
@@ -305,6 +311,9 @@
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="0" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="8" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="0" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="0" hidden="0"/>
     </x:xf>
@@ -314,9 +323,45 @@
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="0" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="0" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="0" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="0" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="6" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="0" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="0" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="7" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="0" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="0" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="0" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="0" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="3" borderId="8" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="0" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="0" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="0" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="0" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="0" hidden="0"/>
     </x:xf>
@@ -344,6 +389,9 @@
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="0" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="8" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="0" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="0" hidden="0"/>
     </x:xf>
@@ -351,126 +399,6 @@
       <x:protection locked="0" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="8" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="14" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="6" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="7" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="8" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="14" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="6" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="7" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="8" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="14" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="6" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="7" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="8" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="0" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -561,11 +489,11 @@
       <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="0" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="0" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="0" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="0" hidden="0"/>
     </x:xf>
@@ -602,19 +530,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela2" displayName="Tabela2" ref="H1:K33" totalsRowShown="0">
-  <x:tableColumns count="4">
-    <x:tableColumn id="1" name="STATUS"/>
-    <x:tableColumn id="2" name="DIR. DE ARQUIVOS"/>
-    <x:tableColumn id="3" name="STATUS REL. ANALITICO"/>
-    <x:tableColumn id="4" name="OBSERVAÇÕES"/>
-  </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleDark8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</x:table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela1" displayName="Tabela1" ref="A1:G27" totalsRowShown="0">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:G27" totalsRowShown="0">
   <x:tableColumns count="7">
     <x:tableColumn id="1" name="CNPJ"/>
     <x:tableColumn id="2" name="NOME EMPRESA"/>
@@ -625,6 +541,18 @@
     <x:tableColumn id="7" name="DATA MOVIMENTO"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</x:table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="H1:K33" totalsRowShown="0">
+  <x:tableColumns count="4">
+    <x:tableColumn id="1" name="STATUS"/>
+    <x:tableColumn id="2" name="DIR. DE ARQUIVOS"/>
+    <x:tableColumn id="3" name="STATUS REL. ANALITICO"/>
+    <x:tableColumn id="4" name="OBSERVAÇÕES"/>
+  </x:tableColumns>
+  <x:tableStyleInfo name="TableStyleDark8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
@@ -930,8 +858,8 @@
   </x:sheetPr>
   <x:dimension ref="A1:N26"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <x:selection activeCell="I7" sqref="I7 I7:I7 I7:I8"/>
+    <x:sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <x:selection activeCell="H5" sqref="H5 H5:H5"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,7 +939,7 @@
       <x:c r="I2" s="16" t="s"/>
       <x:c r="J2" s="16" t="s"/>
       <x:c r="K2" s="16" t="s"/>
-      <x:c r="M2" s="17" t="s"/>
+      <x:c r="M2" s="18" t="s"/>
       <x:c r="N2" s="2" t="s"/>
     </x:row>
     <x:row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1031,34 +959,60 @@
         <x:v>44621</x:v>
       </x:c>
       <x:c r="H3" s="16" t="s">
-        <x:v>21</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="I3" s="16" t="s"/>
       <x:c r="J3" s="16" t="s"/>
       <x:c r="K3" s="16" t="s"/>
-      <x:c r="M3" s="17" t="s"/>
+      <x:c r="M3" s="18" t="s"/>
       <x:c r="N3" s="2" t="s"/>
     </x:row>
     <x:row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <x:c r="G4" s="16" t="s"/>
+      <x:c r="A4" s="15" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B4" s="15" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C4" s="15" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D4" s="15" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E4" s="15" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="G4" s="16">
+        <x:v>44621</x:v>
+      </x:c>
       <x:c r="H4" s="16" t="s">
-        <x:v>21</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="I4" s="16" t="s"/>
       <x:c r="J4" s="16" t="s"/>
       <x:c r="K4" s="16" t="s"/>
-      <x:c r="M4" s="17" t="s"/>
+      <x:c r="M4" s="18" t="s"/>
       <x:c r="N4" s="2" t="s"/>
     </x:row>
     <x:row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="15" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B5" s="15" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C5" s="15" t="s">
+        <x:v>15</x:v>
+      </x:c>
       <x:c r="G5" s="16" t="s"/>
       <x:c r="H5" s="16" t="s">
-        <x:v>21</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="I5" s="16" t="s"/>
       <x:c r="J5" s="16" t="s"/>
       <x:c r="K5" s="16" t="s"/>
-      <x:c r="M5" s="18" t="s"/>
+      <x:c r="M5" s="17" t="s"/>
       <x:c r="N5" s="1" t="s"/>
     </x:row>
     <x:row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1082,7 +1036,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="N8" s="3" t="s">
-        <x:v>22</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1095,7 +1049,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="N9" s="4" t="s">
-        <x:v>23</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1108,7 +1062,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="N10" s="4" t="s">
-        <x:v>24</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1121,7 +1075,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="N11" s="4" t="s">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1134,7 +1088,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="N12" s="4" t="s">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1147,7 +1101,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="N13" s="5" t="s">
-        <x:v>26</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>